<commit_message>
Table 1 and A1
Finished 2 tables... congrats!
</commit_message>
<xml_diff>
--- a/Replication Process.xlsx
+++ b/Replication Process.xlsx
@@ -242,7 +242,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,12 +276,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -386,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -394,9 +388,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -407,41 +398,14 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -449,23 +413,17 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -473,39 +431,72 @@
     <xf numFmtId="18" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -796,7 +787,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -811,63 +802,63 @@
     <col min="8" max="8" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="19" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:8" s="9" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="17" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-    </row>
-    <row r="2" spans="1:8" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+    </row>
+    <row r="2" spans="1:8" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="27" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -877,77 +868,77 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="12" t="s">
+    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="9" t="s">
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="9" t="s">
+    <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="40"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="21" t="s">
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9" t="s">
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="6" t="s">
         <v>29</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="22" t="s">
+    <row r="7" spans="1:8" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -957,114 +948,120 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="22" t="s">
+    <row r="9" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="4" t="s">
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="19" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+    <row r="10" spans="1:8" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="4" t="s">
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="3" t="s">
+    <row r="11" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4" t="s">
+    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4" t="s">
+    <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="21" t="s">
+    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="6" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="F11:F14"/>
     <mergeCell ref="E3:E6"/>
@@ -1073,12 +1070,6 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1102,279 +1093,279 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="16" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="29">
+      <c r="A2" s="17">
         <v>0.25</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="29">
+      <c r="A3" s="17">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="29">
+      <c r="A4" s="17">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="25"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="29">
+      <c r="A5" s="17">
         <v>0.375</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="24"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="29">
+      <c r="A6" s="17">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="29">
+      <c r="A7" s="17">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="29">
+      <c r="A8" s="17">
         <v>0.5</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="25" t="s">
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26" t="s">
+      <c r="G8" s="14"/>
+      <c r="H8" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="29">
+      <c r="A9" s="17">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="25" t="s">
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26" t="s">
+      <c r="G9" s="14"/>
+      <c r="H9" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="29">
+      <c r="A10" s="17">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25" t="s">
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="26" t="s">
+      <c r="H10" s="15" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="29">
+      <c r="A11" s="17">
         <v>0.625</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="26" t="s">
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="15" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="29">
+      <c r="A12" s="17">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="26" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="26" t="s">
+      <c r="H12" s="15" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="29">
+      <c r="A13" s="17">
         <v>0.70833333333333404</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="26" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="29">
+      <c r="A14" s="17">
         <v>0.75</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="29">
+      <c r="A15" s="17">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="41" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="41" t="s">
+      <c r="F15" s="14"/>
+      <c r="G15" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="25"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="29">
+      <c r="A16" s="17">
         <v>0.83333333333333404</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="41" t="s">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="41" t="s">
+      <c r="F16" s="14"/>
+      <c r="G16" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="25"/>
-    </row>
-    <row r="17" spans="4:8" s="37" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="4:8" s="21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37" t="s">
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Push to the deadline
</commit_message>
<xml_diff>
--- a/Replication Process.xlsx
+++ b/Replication Process.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20341"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\LaborIIreplicatation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cl3852\Documents\GitHub\LaborIIreplicatation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BD7256-B426-4EB3-BB98-B3BD662C80A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9684"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="1" r:id="rId1"/>
     <sheet name="Spring sem" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>Figures</t>
   </si>
@@ -171,31 +172,33 @@
     <t>Lab</t>
   </si>
   <si>
-    <t xml:space="preserve">
-NBER
-</t>
-  </si>
-  <si>
-    <t>*下午可以去QC</t>
-  </si>
-  <si>
-    <t>*下午可以去NYU</t>
-  </si>
-  <si>
-    <t>*上午可以去QC</t>
-  </si>
-  <si>
     <t>Spring 2020</t>
   </si>
   <si>
     <t>from REStat package</t>
+  </si>
+  <si>
+    <t>Urban App of GIS</t>
+  </si>
+  <si>
+    <t>QC / NYU / 
+Reading Group</t>
+  </si>
+  <si>
+    <t>QC / NYU</t>
+  </si>
+  <si>
+    <t>*上午可以QC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Race schedule is minimized: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,14 +225,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -241,8 +236,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,31 +302,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor rgb="FF9751CB"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF66FFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -388,10 +391,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -418,40 +421,24 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="18" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="18" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -471,31 +458,88 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -506,8 +550,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF9751CB"/>
+      <color rgb="FFFFA3A3"/>
+      <color rgb="FFFFC1C1"/>
+      <color rgb="FFFF9393"/>
       <color rgb="FF66FFFF"/>
-      <color rgb="FFFF9393"/>
     </mruColors>
   </colors>
   <extLst>
@@ -783,40 +830,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.21875" customWidth="1"/>
-    <col min="4" max="4" width="21.21875" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.77734375" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" customWidth="1"/>
-    <col min="8" max="8" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:8" s="9" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="26" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-    </row>
-    <row r="2" spans="1:8" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
@@ -842,11 +889,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -855,48 +902,48 @@
       <c r="D3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
+        <v>49</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
+        <v>49</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="6" t="s">
         <v>19</v>
       </c>
@@ -904,11 +951,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
+    <row r="6" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="16" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -917,18 +964,18 @@
       <c r="D6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="6" t="s">
         <v>29</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="11" t="s">
         <v>27</v>
       </c>
@@ -945,14 +992,14 @@
         <v>22</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -961,92 +1008,92 @@
       <c r="D8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="21" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="9" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="16" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
       <c r="G13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="6" t="s">
         <v>19</v>
       </c>
@@ -1056,6 +1103,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="F11:F14"/>
     <mergeCell ref="E3:E6"/>
@@ -1064,12 +1117,6 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1077,313 +1124,299 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="16.44140625" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="14" style="28" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="29"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="29"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>0.375</v>
+      </c>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="29"/>
+      <c r="H7" s="30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="32"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>0.625</v>
+      </c>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="38"/>
+      <c r="H10" s="31"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="32"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>0.70833333333333404</v>
+      </c>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="17">
-        <v>0.25</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="17">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="17">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="14"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="17">
-        <v>0.375</v>
-      </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="13"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="17">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="14"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="17">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="17">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="17">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="17">
-        <v>0.625</v>
-      </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="17">
-        <v>0.66666666666666696</v>
-      </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="17">
-        <v>0.70833333333333404</v>
-      </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="17">
+      <c r="E12" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="31"/>
+      <c r="G12" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="29"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
         <v>0.75</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="17">
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="29"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="25" t="s">
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="25" t="s">
+      <c r="F14" s="31"/>
+      <c r="G14" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="14"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="17">
+      <c r="H14" s="29"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
         <v>0.83333333333333404</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="H16" s="14"/>
-    </row>
-    <row r="17" spans="4:8" s="21" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D18" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" t="s">
-        <v>50</v>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="29"/>
+    </row>
+    <row r="16" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="1:8" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="E4:E13"/>
-    <mergeCell ref="D4:D13"/>
-    <mergeCell ref="C4:C13"/>
-    <mergeCell ref="B4:B13"/>
-    <mergeCell ref="G3:G6"/>
+  <mergeCells count="15">
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="D3:D10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="C3:C12"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="E3:E10"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed table e4's code
</commit_message>
<xml_diff>
--- a/Replication Process.xlsx
+++ b/Replication Process.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\LaborIIreplicatation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuxi\Documents\GitHub\LaborIIreplicatation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E0122D-8EC1-44C5-B3B4-9A4894D4A756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9696"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="1" r:id="rId1"/>
@@ -178,7 +179,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -277,12 +278,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9393"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -296,6 +291,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC1C1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -393,12 +394,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="18" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -439,12 +434,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -457,34 +452,46 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -493,35 +500,26 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,9 +529,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFC1C1"/>
       <color rgb="FF9751CB"/>
       <color rgb="FFFFA3A3"/>
-      <color rgb="FFFFC1C1"/>
       <color rgb="FFFF9393"/>
       <color rgb="FF66FFFF"/>
     </mruColors>
@@ -811,40 +809,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:F14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" customWidth="1"/>
-    <col min="8" max="8" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:8" s="8" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="26" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-    </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" spans="1:8" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
@@ -870,11 +868,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="27" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -883,60 +881,60 @@
       <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="49" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
+    <row r="4" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="5" t="s">
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="49" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
+    <row r="5" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="5" t="s">
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="51" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
+    <row r="6" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="24" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -945,28 +943,28 @@
       <c r="D6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="5" t="s">
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="49" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="10" t="s">
+    <row r="7" spans="1:8" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -976,11 +974,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="27" t="s">
+    <row r="8" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="24" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -990,9 +988,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+    <row r="9" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
       <c r="G9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1000,9 +998,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+    <row r="10" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
       <c r="G10" s="3" t="s">
         <v>17</v>
       </c>
@@ -1010,11 +1008,11 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E11" s="27" t="s">
+    <row r="11" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="24" t="s">
         <v>20</v>
       </c>
       <c r="G11" s="4" t="s">
@@ -1024,9 +1022,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
+    <row r="12" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="3" t="s">
         <v>18</v>
       </c>
@@ -1034,9 +1032,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
+    <row r="13" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1044,9 +1042,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
+    <row r="14" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
       <c r="G14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1056,18 +1054,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="F11:F14"/>
     <mergeCell ref="E3:E6"/>
     <mergeCell ref="F3:F6"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1075,291 +1073,284 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="14" style="18" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="14" style="16" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="12">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="19"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+      <c r="F3" s="17"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="17"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
         <v>0.375</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="19"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="17"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="19"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="17"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
         <v>0.5</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="42" t="s">
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="36" t="s">
+      <c r="G7" s="17"/>
+      <c r="H7" s="38" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="12">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="37"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="12">
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="39"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="42" t="s">
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="36" t="s">
+      <c r="H9" s="38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="12">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
         <v>0.625</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="36" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="43"/>
-      <c r="H10" s="38"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="12">
+      <c r="G10" s="45"/>
+      <c r="H10" s="40"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="37"/>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12">
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="39"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
         <v>0.70833333333333404</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="49" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="50" t="s">
+      <c r="F12" s="40"/>
+      <c r="G12" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="19"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
+      <c r="H12" s="17"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
         <v>0.75</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="19"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="17"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
         <v>0.79166666666666696</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="50" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="52" t="s">
+      <c r="F14" s="40"/>
+      <c r="G14" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="19"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="12">
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
         <v>0.83333333333333404</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="19"/>
-    </row>
-    <row r="16" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-    </row>
-    <row r="17" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="17"/>
+    </row>
+    <row r="16" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C3:C12"/>
-    <mergeCell ref="B3:B12"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="E3:E10"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="D12:D13"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="H9:H11"/>
     <mergeCell ref="D3:D10"/>
@@ -1368,6 +1359,13 @@
     <mergeCell ref="F10:F15"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="G14:G15"/>
+    <mergeCell ref="C3:C12"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="E3:E10"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>